<commit_message>
update: Se actualiza proyecto
</commit_message>
<xml_diff>
--- a/TestChoucair/DataTest.xlsx
+++ b/TestChoucair/DataTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuri\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuri\OneDrive\Documentos\GitHub\TestChoucair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72084D28-FAB0-40B5-AAD1-F0A04D7FE94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E487104F-7AD9-4107-BE37-03F78F697145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08DE13AF-EE96-4B7B-AB12-102E0122649A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>nombre</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>carlos@gmail.com</t>
+  </si>
+  <si>
+    <t>contraseña</t>
+  </si>
+  <si>
+    <t>confirmar contraseña</t>
+  </si>
+  <si>
+    <t>Colombia1990.</t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -112,16 +121,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -437,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CE890B-5763-49CC-9147-90C5F4C08343}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,28 +482,42 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>